<commit_message>
updating syncopation stims w/ degrees
</commit_message>
<xml_diff>
--- a/stimuli/witek_stim/ELS_stimbreakdown.xlsx
+++ b/stimuli/witek_stim/ELS_stimbreakdown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathios.n/Documents/Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickkathios/Documents/Research/TEAM/stimuli/witek_stim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095881CE-1F58-894C-87AC-8BBB87AC095E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B0991-D338-3648-9F96-BB7F49DDCAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="500" windowWidth="10000" windowHeight="17440" xr2:uid="{491A8713-495B-B147-B8F6-CD033583D7BD}"/>
+    <workbookView xWindow="22720" yWindow="500" windowWidth="12360" windowHeight="17440" xr2:uid="{491A8713-495B-B147-B8F6-CD033583D7BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>stim_name</t>
   </si>
   <si>
-    <t>syncopation_degree</t>
-  </si>
-  <si>
     <t>syncopation_group</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Honeydippers - Impeach the president.mp3</t>
+  </si>
+  <si>
+    <t>syncopation_level</t>
   </si>
 </sst>
 </file>
@@ -456,14 +456,17 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -472,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -480,13 +483,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -494,13 +497,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -508,13 +511,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -522,13 +525,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -536,13 +539,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -550,13 +553,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -564,13 +567,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
         <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -578,13 +581,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -592,13 +595,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -606,13 +609,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -620,13 +623,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
         <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,13 +637,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
         <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,13 +651,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
         <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -662,13 +665,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -676,19 +679,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
         <v>81</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D16">
-    <sortCondition ref="C1:C16"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>